<commit_message>
test name values updates
</commit_message>
<xml_diff>
--- a/Data Files/reviewURLs.xlsx
+++ b/Data Files/reviewURLs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" firstSheet="7" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" firstSheet="10" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="allPages" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="729" uniqueCount="369">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="369">
   <si>
     <t>https://www.review.lexus.com</t>
   </si>
@@ -3956,201 +3956,156 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A38"/>
+  <dimension ref="A1:A29"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="G50" sqref="G50"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>123</v>
+        <v>132</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>126</v>
+        <v>135</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>128</v>
+        <v>137</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>129</v>
+        <v>138</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>131</v>
+        <v>140</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>132</v>
+        <v>141</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>133</v>
+        <v>142</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>134</v>
+        <v>143</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>136</v>
+        <v>145</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>138</v>
+        <v>147</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>139</v>
+        <v>148</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>140</v>
+        <v>149</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
         <v>150</v>
       </c>
     </row>
@@ -5268,7 +5223,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:A5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
FAD, dealers, FCV CEPO URL updates
</commit_message>
<xml_diff>
--- a/Data Files/reviewURLs.xlsx
+++ b/Data Files/reviewURLs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="allPages" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="722" uniqueCount="382">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="395">
   <si>
     <t>https://www.review.lexus.com</t>
   </si>
@@ -1154,15 +1154,6 @@
     <t>https://staging.lexus.com/$#@$</t>
   </si>
   <si>
-    <t>https://staging.lexus.com/dealers/60419-keyes-lexus</t>
-  </si>
-  <si>
-    <t>https://staging.lexus.com/dealers/60406-lexus-santa-monica</t>
-  </si>
-  <si>
-    <t>https://staging.lexus.com/dealers/60445-lexus-of-cerritos</t>
-  </si>
-  <si>
     <t>https://stg-lcom.cdn.cepo-proxy.tms.aws.lexus.com/concept/LFSA/</t>
   </si>
   <si>
@@ -1191,6 +1182,54 @@
   </si>
   <si>
     <t>https://stg-lcom.cdn.cepo-proxy.tms.aws.lexus.com/concept/LF-30-Electrified</t>
+  </si>
+  <si>
+    <t>https://stg-lcom.cdn.cepo-proxy.tms.aws.lexus.com/about</t>
+  </si>
+  <si>
+    <t>https://stg-lcom.cdn.cepo-proxy.tms.aws.lexus.com/about/manufacturing</t>
+  </si>
+  <si>
+    <t>https://stg-lcom.cdn.cepo-proxy.tms.aws.lexus.com/about/technology</t>
+  </si>
+  <si>
+    <t>https://stg-lcom.cdn.cepo-proxy.tms.aws.lexus.com/about/environment</t>
+  </si>
+  <si>
+    <t>https://stg-lcom.cdn.cepo-proxy.tms.aws.lexus.com/about/philanthropy</t>
+  </si>
+  <si>
+    <t>https://stg-lcom.cdn.cepo-proxy.tms.aws.lexus.com/accessibility</t>
+  </si>
+  <si>
+    <t>https://stg-lcom.cdn.cepo-proxy.tms.aws.lexus.com/careers</t>
+  </si>
+  <si>
+    <t>https://stg-lcom.cdn.cepo-proxy.tms.aws.lexus.com/privacy</t>
+  </si>
+  <si>
+    <t>https://stg-lcom.cdn.cepo-proxy.tms.aws.lexus.com/dealers</t>
+  </si>
+  <si>
+    <t>https://stg-lcom.cdn.cepo-proxy.tms.aws.lexus.com/dealers/63110-lexus-of-manhattan</t>
+  </si>
+  <si>
+    <t>https://stg-lcom.cdn.cepo-proxy.tms.aws.lexus.com/dealers/64204-sewell-lexus</t>
+  </si>
+  <si>
+    <t>https://stg-lcom.cdn.cepo-proxy.tms.aws.lexus.com/dealers/61230-mcgrath-lexus-of-chicago</t>
+  </si>
+  <si>
+    <t>https://stg-lcom.cdn.cepo-proxy.tms.aws.lexus.com/dealers/60438-jim-falk-lexus-of-beverly-hills</t>
+  </si>
+  <si>
+    <t>https://stg-lcom.cdn.cepo-proxy.tms.aws.lexus.com/dealers/60419-keyes-lexus</t>
+  </si>
+  <si>
+    <t>https://stg-lcom.cdn.cepo-proxy.tms.aws.lexus.com/dealers/60406-lexus-santa-monica</t>
+  </si>
+  <si>
+    <t>https://stg-lcom.cdn.cepo-proxy.tms.aws.lexus.com/dealers/60445-lexus-of-cerritos</t>
   </si>
 </sst>
 </file>
@@ -4496,10 +4535,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A28"/>
+  <dimension ref="A1:A26"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31:XFD39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4511,27 +4550,27 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>324</v>
+        <v>379</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>325</v>
+        <v>380</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>326</v>
+        <v>381</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>327</v>
+        <v>382</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>328</v>
+        <v>383</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.45">
@@ -4541,106 +4580,96 @@
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>330</v>
+        <v>384</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>331</v>
+        <v>385</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>332</v>
+        <v>386</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>333</v>
+        <v>336</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>334</v>
+        <v>337</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>343</v>
+        <v>359</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>345</v>
+        <v>360</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A27" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A28" t="s">
         <v>366</v>
       </c>
     </row>
@@ -5017,7 +5046,7 @@
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
     </row>
   </sheetData>
@@ -5033,7 +5062,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
@@ -5140,54 +5169,64 @@
   <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:A8"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A1" t="s">
-        <v>317</v>
+      <c r="A1" s="1" t="s">
+        <v>387</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
-        <v>318</v>
+      <c r="A2" s="1" t="s">
+        <v>388</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
-        <v>319</v>
+      <c r="A3" s="1" t="s">
+        <v>389</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
-        <v>320</v>
+      <c r="A4" s="1" t="s">
+        <v>390</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
-        <v>321</v>
+      <c r="A5" s="1" t="s">
+        <v>391</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
-        <v>369</v>
+      <c r="A6" s="1" t="s">
+        <v>392</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
-        <v>370</v>
+      <c r="A7" s="1" t="s">
+        <v>393</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
-        <v>371</v>
+      <c r="A8" s="1" t="s">
+        <v>394</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1"/>
+    <hyperlink ref="A2" r:id="rId2"/>
+    <hyperlink ref="A3" r:id="rId3"/>
+    <hyperlink ref="A4" r:id="rId4"/>
+    <hyperlink ref="A5" r:id="rId5"/>
+    <hyperlink ref="A6" r:id="rId6"/>
+    <hyperlink ref="A7" r:id="rId7"/>
+    <hyperlink ref="A8" r:id="rId8"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId9"/>
 </worksheet>
 </file>
 
@@ -5226,34 +5265,34 @@
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
-        <v>381</v>
+      <c r="A5" s="1" t="s">
+        <v>378</v>
       </c>
     </row>
   </sheetData>
@@ -5262,9 +5301,10 @@
     <hyperlink ref="A2" r:id="rId2"/>
     <hyperlink ref="A3" r:id="rId3"/>
     <hyperlink ref="A4" r:id="rId4"/>
+    <hyperlink ref="A5" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId5"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId6"/>
 </worksheet>
 </file>
 
@@ -5305,22 +5345,22 @@
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
     </row>
   </sheetData>

</xml_diff>